<commit_message>
bugfix boxplot-dit-swarm labels var
</commit_message>
<xml_diff>
--- a/output/CD-3_dados_pesquisa_opiniao_produto.xlsx
+++ b/output/CD-3_dados_pesquisa_opiniao_produto.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>